<commit_message>
uploaded transfered-learning model and result logs
</commit_message>
<xml_diff>
--- a/Fine-Tuning-Logs/LSTM_Encoder_Decoder_Close+Indicators_.xlsx
+++ b/Fine-Tuning-Logs/LSTM_Encoder_Decoder_Close+Indicators_.xlsx
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -172,6 +172,9 @@
     <xf borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="2" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,27 +732,27 @@
       <c r="F13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="13">
         <f t="shared" ref="G13:L13" si="1">AVERAGE(G2:G11)</f>
         <v>0.1398873031</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="13">
         <f t="shared" si="1"/>
         <v>1011.465588</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="13">
         <f t="shared" si="1"/>
         <v>0.1432222426</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="13">
         <f t="shared" si="1"/>
         <v>1035.578967</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="13">
         <f t="shared" si="1"/>
         <v>0.3703135014</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="13">
         <f t="shared" si="1"/>
         <v>-0.2181811243</v>
       </c>
@@ -763,27 +766,27 @@
       <c r="F14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="13">
         <f t="shared" ref="G14:L14" si="2">STDEV(G2:G11)</f>
         <v>0.06589197722</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="13">
         <f t="shared" si="2"/>
         <v>476.4368485</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="13">
         <f t="shared" si="2"/>
         <v>0.001896321812</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="13">
         <f t="shared" si="2"/>
         <v>13.7114808</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="13">
         <f t="shared" si="2"/>
         <v>0.1235602978</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="13">
         <f t="shared" si="2"/>
         <v>0.04638959372</v>
       </c>

</xml_diff>